<commit_message>
add a csv file
add a csv file
</commit_message>
<xml_diff>
--- a/Murphy-Machine-Learning-print-typos.xlsx
+++ b/Murphy-Machine-Learning-print-typos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Guozi/ML/Books@ML/ML-Errara/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Guozi/Github/Machine_Learning/Murphy-Machine-Learning-A-Probabilistic-Perspective-Errata-and-Notes-4th-printings/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="211">
   <si>
     <t>Page</t>
   </si>
@@ -648,6 +648,15 @@
   </si>
   <si>
     <t>so it need</t>
+  </si>
+  <si>
+    <t>24.3.3</t>
+  </si>
+  <si>
+    <t>spread</t>
+  </si>
+  <si>
+    <t>spreads</t>
   </si>
 </sst>
 </file>
@@ -997,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="H77" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2036,21 +2045,41 @@
         <v>104</v>
       </c>
       <c r="B77" s="1">
+        <v>852</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D77" s="1">
+        <v>2</v>
+      </c>
+      <c r="E77" s="1">
+        <v>1</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B78" s="1">
         <v>871</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C78" s="1">
         <v>24.6</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D78" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E77" s="1">
+      <c r="E78" s="1">
         <v>3</v>
       </c>
-      <c r="F77" s="1" t="s">
+      <c r="F78" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G77" s="1" t="s">
+      <c r="G78" s="1" t="s">
         <v>128</v>
       </c>
     </row>

</xml_diff>